<commit_message>
added anti aliasing LP to adc
</commit_message>
<xml_diff>
--- a/Rev1/Release/Released/BOM/Bill of Materials-DAQ_1.xlsx
+++ b/Rev1/Release/Released/BOM/Bill of Materials-DAQ_1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>Description</t>
   </si>
@@ -51,6 +51,15 @@
     <t>C0603C104M4RACTU</t>
   </si>
   <si>
+    <t>CAP CER 0.18UF 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>C8, C9</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R7BB184</t>
+  </si>
+  <si>
     <t>LED GREEN CLEAR 0603 SMD</t>
   </si>
   <si>
@@ -166,6 +175,15 @@
   </si>
   <si>
     <t>RC0603FR-072K2L</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>R23, R24</t>
+  </si>
+  <si>
+    <t>CRCW06031K00FKEA</t>
   </si>
   <si>
     <t>IC REG LIN 3.3V 800MA SOT223-3</t>
@@ -541,7 +559,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView view="normal" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" sqref="A1"/>
@@ -603,7 +621,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>13</v>
@@ -645,7 +663,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D7" s="49" t="s">
         <v>22</v>
@@ -659,7 +677,7 @@
         <v>24</v>
       </c>
       <c r="C8" s="50">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="49" t="s">
         <v>25</v>
@@ -689,21 +707,21 @@
       <c r="C10" s="50">
         <v>1</v>
       </c>
-      <c r="D10" s="49"/>
+      <c r="D10" s="49" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B11" s="49" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="50">
         <v>1</v>
       </c>
-      <c r="D11" s="49" t="s">
-        <v>33</v>
-      </c>
+      <c r="D11" s="49"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="48" t="s">
@@ -713,35 +731,35 @@
         <v>35</v>
       </c>
       <c r="C12" s="50">
-        <v>12</v>
-      </c>
-      <c r="D12" s="49"/>
+        <v>1</v>
+      </c>
+      <c r="D12" s="49" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="50">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D13" s="49"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B14" s="49" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C14" s="50">
-        <v>9</v>
-      </c>
-      <c r="D14" s="49" t="s">
-        <v>40</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D14" s="49"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="48" t="s">
@@ -751,7 +769,7 @@
         <v>42</v>
       </c>
       <c r="C15" s="50">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D15" s="49" t="s">
         <v>43</v>
@@ -765,7 +783,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="50">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="D16" s="49" t="s">
         <v>46</v>
@@ -807,28 +825,32 @@
         <v>54</v>
       </c>
       <c r="C19" s="50">
-        <v>1</v>
-      </c>
-      <c r="D19" s="49"/>
+        <v>2</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="48" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B20" s="49" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C20" s="50">
         <v>1</v>
       </c>
-      <c r="D20" s="49"/>
+      <c r="D20" s="49" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="48" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B21" s="49" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C21" s="50">
         <v>1</v>
@@ -837,15 +859,39 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="48" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B22" s="49" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" s="50">
         <v>1</v>
       </c>
       <c r="D22" s="49"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="50">
+        <v>1</v>
+      </c>
+      <c r="D23" s="49"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="50">
+        <v>1</v>
+      </c>
+      <c r="D24" s="49"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>